<commit_message>
Delivery Note test cases updated
</commit_message>
<xml_diff>
--- a/tests/artifact/data/DeliveryNote.data.xlsx
+++ b/tests/artifact/data/DeliveryNote.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>schema.path</t>
   </si>
@@ -143,6 +143,108 @@
   </si>
   <si>
     <t>227</t>
+  </si>
+  <si>
+    <t>orgtype</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>yearstart</t>
+  </si>
+  <si>
+    <t>01-04-2023</t>
+  </si>
+  <si>
+    <t>yearend</t>
+  </si>
+  <si>
+    <t>01-03-2024</t>
+  </si>
+  <si>
+    <t>orgstate</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>orgcity</t>
+  </si>
+  <si>
+    <t>Banglore</t>
+  </si>
+  <si>
+    <t>orgaddr</t>
+  </si>
+  <si>
+    <t>Business bay banglore near IT park</t>
+  </si>
+  <si>
+    <t>orgpincode</t>
+  </si>
+  <si>
+    <t>411023</t>
+  </si>
+  <si>
+    <t>orgcountry</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>invflag</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>invsflag</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>billflag</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>avflag</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>invaliddcidname</t>
+  </si>
+  <si>
+    <t>@#@@#,"   ",WQWE@#@#</t>
+  </si>
+  <si>
+    <t>invalidcustid</t>
+  </si>
+  <si>
+    <t>757,574,274</t>
+  </si>
+  <si>
+    <t>invaliddcno</t>
+  </si>
+  <si>
+    <t>102,110,232</t>
+  </si>
+  <si>
+    <t>invaliddcflag</t>
+  </si>
+  <si>
+    <t>0,1,0</t>
+  </si>
+  <si>
+    <t>invalidtaxstate</t>
+  </si>
+  <si>
+    <t>maha,GJ,MP</t>
   </si>
 </sst>
 </file>
@@ -150,10 +252,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -660,16 +762,16 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1243,7 +1345,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
@@ -1414,56 +1516,141 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A23" s="5"/>
-    </row>
-    <row r="24" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A25" s="5"/>
-    </row>
-    <row r="26" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A34" s="5"/>
-    </row>
-    <row r="35" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A35" s="5"/>
-    </row>
-    <row r="36" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A38" s="5"/>
+    <row r="22" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="39" ht="23.1" customHeight="1" spans="1:1">
       <c r="A39" s="5"/>
@@ -1651,68 +1838,84 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0" objects="1"/>
   <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="14" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="13" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="11" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A13,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="16">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="15" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="4">
+      <formula>LEN(TRIM(B30))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="7" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A7,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A7,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="5" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A7,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="10">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B33">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
+      <formula>LEN(TRIM(B31))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A6 A9:A12 A14:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="13" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="17" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="14" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="15" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="19" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="20" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E6 C7:E8 B9:E12 B14:E1048576 C13:E13">
-    <cfRule type="expression" dxfId="5" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E6 C7:E8 B9:E12 B14:E29 C30:E33 B34:E1048576 C13:E13">
+    <cfRule type="expression" dxfId="5" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="24">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Branch Name: NegativeTcDelivery: Delivery Note Negative test cases
</commit_message>
<xml_diff>
--- a/tests/artifact/data/DeliveryNote.data.xlsx
+++ b/tests/artifact/data/DeliveryNote.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>schema.path</t>
   </si>
@@ -143,6 +143,108 @@
   </si>
   <si>
     <t>227</t>
+  </si>
+  <si>
+    <t>orgtype</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>yearstart</t>
+  </si>
+  <si>
+    <t>01-04-2023</t>
+  </si>
+  <si>
+    <t>yearend</t>
+  </si>
+  <si>
+    <t>01-03-2024</t>
+  </si>
+  <si>
+    <t>orgstate</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>orgcity</t>
+  </si>
+  <si>
+    <t>Banglore</t>
+  </si>
+  <si>
+    <t>orgaddr</t>
+  </si>
+  <si>
+    <t>Business bay banglore near IT park</t>
+  </si>
+  <si>
+    <t>orgpincode</t>
+  </si>
+  <si>
+    <t>411023</t>
+  </si>
+  <si>
+    <t>orgcountry</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>invflag</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>invsflag</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>billflag</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>avflag</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>invaliddcidname</t>
+  </si>
+  <si>
+    <t>@#@@#,"   ",WQWE@#@#</t>
+  </si>
+  <si>
+    <t>invalidcustid</t>
+  </si>
+  <si>
+    <t>757,574,274</t>
+  </si>
+  <si>
+    <t>invaliddcno</t>
+  </si>
+  <si>
+    <t>102,110,232</t>
+  </si>
+  <si>
+    <t>invaliddcflag</t>
+  </si>
+  <si>
+    <t>0,1,0</t>
+  </si>
+  <si>
+    <t>invalidtaxstate</t>
+  </si>
+  <si>
+    <t>maha,GJ,MP</t>
   </si>
 </sst>
 </file>
@@ -150,10 +252,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -660,16 +762,16 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1243,7 +1345,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
@@ -1414,56 +1516,141 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A23" s="5"/>
-    </row>
-    <row r="24" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A25" s="5"/>
-    </row>
-    <row r="26" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A34" s="5"/>
-    </row>
-    <row r="35" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A35" s="5"/>
-    </row>
-    <row r="36" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A38" s="5"/>
+    <row r="22" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="39" ht="23.1" customHeight="1" spans="1:1">
       <c r="A39" s="5"/>
@@ -1651,68 +1838,84 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0" objects="1"/>
   <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="14" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="13" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="11" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A13,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="16">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="15" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="4">
+      <formula>LEN(TRIM(B30))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="7" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A7,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A7,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="5" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A7,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="10">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B33">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
+      <formula>LEN(TRIM(B31))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A6 A9:A12 A14:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="13" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="17" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="14" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="15" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="19" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="20" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E6 C7:E8 B9:E12 B14:E1048576 C13:E13">
-    <cfRule type="expression" dxfId="5" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E6 C7:E8 B9:E12 B14:E29 C30:E33 B34:E1048576 C13:E13">
+    <cfRule type="expression" dxfId="5" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="24">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
delivery Test case added with 100% execution rate
</commit_message>
<xml_diff>
--- a/tests/artifact/data/DeliveryNote.data.xlsx
+++ b/tests/artifact/data/DeliveryNote.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>schema.path</t>
   </si>
@@ -245,6 +245,21 @@
   </si>
   <si>
     <t>maha,GJ,MP</t>
+  </si>
+  <si>
+    <t>invalid_dcid</t>
+  </si>
+  <si>
+    <t>custid</t>
+  </si>
+  <si>
+    <t>2566</t>
+  </si>
+  <si>
+    <t>dcno</t>
+  </si>
+  <si>
+    <t>281</t>
   </si>
 </sst>
 </file>
@@ -1344,8 +1359,8 @@
   <sheetPr/>
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
@@ -1652,14 +1667,29 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A40" s="5"/>
-    </row>
-    <row r="41" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A41" s="5"/>
+    <row r="39" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="42" ht="23.1" customHeight="1" spans="1:1">
       <c r="A42" s="5"/>

</xml_diff>